<commit_message>
reduced value of debouncing capacitors C18/C25/C33/C34
</commit_message>
<xml_diff>
--- a/BassOwl-Lite.bom.xlsx
+++ b/BassOwl-Lite.bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\tfa98xx_bt_spkr\kicad5_workspace\projects\BTFA_Rev4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\bassowl-lite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E287F3-DDB2-4D49-9E9C-1B0EF883B722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAAFADB-F149-44CE-AC24-0F1671FAB254}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>Designator</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -36,9 +36,6 @@
     <t>C8,C11</t>
   </si>
   <si>
-    <t>C10,C12,C14,C15,C18,C25,C29,C30,C31,C32,C33,C34</t>
-  </si>
-  <si>
     <t>R1,R5</t>
   </si>
   <si>
@@ -72,24 +69,15 @@
     <t>R9</t>
   </si>
   <si>
-    <t>2k2</t>
-  </si>
-  <si>
     <t>R11,R12</t>
   </si>
   <si>
-    <t>2k</t>
-  </si>
-  <si>
     <t>R13,R14,R15,R16,R21</t>
   </si>
   <si>
     <t>R17</t>
   </si>
   <si>
-    <t>22k</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -337,6 +325,30 @@
   </si>
   <si>
     <t>U3</t>
+  </si>
+  <si>
+    <t>C18,C25,C33,C34</t>
+  </si>
+  <si>
+    <t>0603B681K500NT</t>
+  </si>
+  <si>
+    <t>C10,C12,C14,C15,C29,C30,C31,C32</t>
+  </si>
+  <si>
+    <t>680p / 50V / 0603</t>
+  </si>
+  <si>
+    <t>2k2 / 0603</t>
+  </si>
+  <si>
+    <t>2k / 0603</t>
+  </si>
+  <si>
+    <t>330 / 0603</t>
+  </si>
+  <si>
+    <t>22k / 0603</t>
   </si>
 </sst>
 </file>
@@ -1310,10 +1322,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" customHeight="1"/>
@@ -1330,13 +1342,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
@@ -1344,13 +1356,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C2" s="4">
         <v>3</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
@@ -1358,461 +1370,475 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4">
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C4" s="4">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4">
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="C6" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C7" s="4">
         <v>2</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C8" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="C11" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C13" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C14" s="4">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C15" s="4">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C16" s="4">
         <v>1</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C18" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C19" s="4">
-        <v>5</v>
-      </c>
-      <c r="D19" s="4">
-        <v>330</v>
+        <v>2</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C20" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>21</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="C21" s="4">
         <v>1</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="C22" s="4">
         <v>1</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C23" s="4">
         <v>1</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>93</v>
+        <v>36</v>
       </c>
       <c r="C24" s="4">
         <v>1</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="C25" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="C26" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C27" s="4">
         <v>1</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="C28" s="4">
         <v>1</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="C29" s="4">
         <v>1</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C30" s="4">
         <v>1</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C31" s="4">
         <v>1</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>38</v>
+        <v>28</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="C32" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>57</v>
+        <v>30</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C33" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C34" s="4">
+        <v>1</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1">
+      <c r="A35" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="4">
         <v>2</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1">
-      <c r="A35" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C35" s="1">
-        <v>1</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>103</v>
+      <c r="D35" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" customHeight="1">
+      <c r="A36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>